<commit_message>
Fix graphic and output issues.
</commit_message>
<xml_diff>
--- a/Campus.xlsx
+++ b/Campus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangj\Desktop\CISC320\Lesson 19- Graph Applications\GitHub lesson-19-graph-applications\lesson-19-graph-applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBCBD65-9EA9-4CDC-98DF-B08675B531C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9810A46-D07A-4C11-AFF4-4ADB8B067373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
   <si>
     <t>Ewing Hall</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Alfred Lerner Hall</t>
-  </si>
-  <si>
-    <t>Purnell</t>
   </si>
   <si>
     <t>Amy du Pont Music Building</t>
@@ -431,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,7 +439,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -453,7 +450,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -464,7 +461,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -475,7 +472,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -489,7 +486,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -511,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>130</v>
@@ -522,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>58</v>
@@ -530,7 +527,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -541,10 +538,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
         <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
       </c>
       <c r="C13">
         <v>80</v>
@@ -555,7 +552,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>75</v>
@@ -563,10 +560,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
         <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
       </c>
       <c r="C17">
         <v>79</v>
@@ -577,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>39</v>
@@ -588,7 +585,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>27</v>
@@ -599,7 +596,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>56</v>
@@ -607,10 +604,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>46</v>
@@ -618,10 +615,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>72</v>
@@ -629,10 +626,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27">
         <v>45</v>
@@ -640,10 +637,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28">
         <v>44</v>
@@ -651,10 +648,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
         <v>20</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
       </c>
       <c r="C30">
         <v>47</v>
@@ -662,10 +659,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31">
         <v>50</v>
@@ -673,10 +670,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>120</v>
@@ -684,10 +681,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
         <v>21</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
       </c>
       <c r="C34">
         <v>9</v>
@@ -695,10 +692,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>34</v>
@@ -706,10 +703,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
         <v>24</v>
-      </c>
-      <c r="B37" t="s">
-        <v>25</v>
       </c>
       <c r="C37">
         <v>50</v>
@@ -717,10 +714,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
         <v>25</v>
-      </c>
-      <c r="B39" t="s">
-        <v>26</v>
       </c>
       <c r="C39">
         <v>42</v>
@@ -728,10 +725,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
         <v>27</v>
-      </c>
-      <c r="B41" t="s">
-        <v>28</v>
       </c>
       <c r="C41">
         <v>11</v>
@@ -739,10 +736,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
         <v>10</v>
-      </c>
-      <c r="B43" t="s">
-        <v>11</v>
       </c>
       <c r="C43">
         <v>18</v>
@@ -750,10 +747,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44">
         <v>16</v>
@@ -761,10 +758,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45">
         <v>80</v>
@@ -772,10 +769,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
         <v>15</v>
-      </c>
-      <c r="B47" t="s">
-        <v>16</v>
       </c>
       <c r="C47">
         <v>170</v>
@@ -783,10 +780,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C49">
         <v>55</v>
@@ -794,10 +791,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50">
         <v>28</v>
@@ -805,10 +802,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C52">
         <v>59</v>
@@ -816,10 +813,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C53">
         <v>23</v>
@@ -827,10 +824,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C54">
         <v>58</v>

</xml_diff>